<commit_message>
Updated StatusView, Added Dialog Box to indicate Errors in parsing and when the file is open
</commit_message>
<xml_diff>
--- a/Breeding.xlsx
+++ b/Breeding.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2557" uniqueCount="586">
   <si>
     <t>Ref. No</t>
   </si>
@@ -1640,9 +1640,6 @@
     <t>REJECT</t>
   </si>
   <si>
-    <t>FOURCE DRY</t>
-  </si>
-  <si>
     <t>BAD</t>
   </si>
   <si>
@@ -1701,6 +1698,81 @@
   </si>
   <si>
     <t>Past candidate for reject</t>
+  </si>
+  <si>
+    <t>09381</t>
+  </si>
+  <si>
+    <t>09401</t>
+  </si>
+  <si>
+    <t>09402</t>
+  </si>
+  <si>
+    <t>A321</t>
+  </si>
+  <si>
+    <t>A322</t>
+  </si>
+  <si>
+    <t>A323</t>
+  </si>
+  <si>
+    <t>A324</t>
+  </si>
+  <si>
+    <t>A325</t>
+  </si>
+  <si>
+    <t>A326</t>
+  </si>
+  <si>
+    <t>A327</t>
+  </si>
+  <si>
+    <t>A328</t>
+  </si>
+  <si>
+    <t>A329</t>
+  </si>
+  <si>
+    <t>A330</t>
+  </si>
+  <si>
+    <t>A331</t>
+  </si>
+  <si>
+    <t>A332</t>
+  </si>
+  <si>
+    <t>A333</t>
+  </si>
+  <si>
+    <t>A334</t>
+  </si>
+  <si>
+    <t>A335</t>
+  </si>
+  <si>
+    <t>A336</t>
+  </si>
+  <si>
+    <t>A337</t>
+  </si>
+  <si>
+    <t>A338</t>
+  </si>
+  <si>
+    <t>A339</t>
+  </si>
+  <si>
+    <t>A340</t>
+  </si>
+  <si>
+    <t>BELOW AVERAGE FOURCE DRY</t>
+  </si>
+  <si>
+    <t>FOURCE DRY FOURCE DRY</t>
   </si>
 </sst>
 </file>
@@ -1769,7 +1841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1804,6 +1876,12 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2306,7 +2384,7 @@
   <dimension ref="A1:R357"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2323,11 +2401,12 @@
     <col min="10" max="10" width="20.28515625" style="3" customWidth="1"/>
     <col min="11" max="11" width="25.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" customWidth="1"/>
     <col min="14" max="14" width="22.5703125" customWidth="1"/>
     <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -2367,7 +2446,7 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
@@ -2383,7 +2462,7 @@
         <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
@@ -2405,8 +2484,8 @@
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1">
-        <v>4</v>
+      <c r="I2" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>22</v>
@@ -2418,7 +2497,6 @@
         <f>[Date Breed]+114</f>
         <v>43040</v>
       </c>
-      <c r="M2"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
       <c r="A3" t="s">
@@ -2439,8 +2517,8 @@
       <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="1">
-        <v>4</v>
+      <c r="I3" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>22</v>
@@ -2452,7 +2530,6 @@
         <f>[Date Breed]+114</f>
         <v>43043</v>
       </c>
-      <c r="M3"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
       <c r="A4" t="s">
@@ -2473,8 +2550,8 @@
       <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="1">
-        <v>4</v>
+      <c r="I4" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>27</v>
@@ -2486,7 +2563,6 @@
         <f>[Date Breed]+114</f>
         <v>43045</v>
       </c>
-      <c r="M4"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
       <c r="A5" t="s">
@@ -2507,8 +2583,8 @@
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1">
-        <v>4</v>
+      <c r="I5" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>27</v>
@@ -2520,7 +2596,6 @@
         <f>[Date Breed]+114</f>
         <v>43046</v>
       </c>
-      <c r="M5"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
       <c r="A6" t="s">
@@ -2541,8 +2616,8 @@
       <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="1">
-        <v>4</v>
+      <c r="I6" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>22</v>
@@ -2554,7 +2629,6 @@
         <f>[Date Breed]+114</f>
         <v>43050</v>
       </c>
-      <c r="M6"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
       <c r="A7" t="s">
@@ -2575,8 +2649,8 @@
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="1">
-        <v>3</v>
+      <c r="I7" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>22</v>
@@ -2588,7 +2662,6 @@
         <f>[Date Breed]+114</f>
         <v>43051</v>
       </c>
-      <c r="M7"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
       <c r="A8" t="s">
@@ -2600,6 +2673,9 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8" s="16">
+        <v>43084</v>
+      </c>
       <c r="E8" s="2">
         <v>42939</v>
       </c>
@@ -2609,8 +2685,8 @@
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="1">
-        <v>2</v>
+      <c r="I8" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>36</v>
@@ -2642,6 +2718,9 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
+      <c r="D9" s="16">
+        <v>43084</v>
+      </c>
       <c r="E9" s="2">
         <v>42940</v>
       </c>
@@ -2651,8 +2730,8 @@
       <c r="H9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="1">
-        <v>2</v>
+      <c r="I9" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>36</v>
@@ -2684,6 +2763,9 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
+      <c r="D10" s="16">
+        <v>43084</v>
+      </c>
       <c r="E10" s="2">
         <v>42942</v>
       </c>
@@ -2693,8 +2775,8 @@
       <c r="H10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="1">
-        <v>4</v>
+      <c r="I10" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>36</v>
@@ -2735,8 +2817,8 @@
       <c r="H11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="1">
-        <v>3</v>
+      <c r="I11" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>36</v>
@@ -2755,52 +2837,56 @@
         <v>4</v>
       </c>
       <c r="Q11" t="s">
-        <v>537</v>
+        <v>584</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" t="s">
+      <c r="A12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="C12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="27">
         <v>42943</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="F12" s="26"/>
+      <c r="G12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27">
         <f>[Date Breed]+114</f>
         <v>43057</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="29">
         <v>43057</v>
       </c>
-      <c r="O12" t="s">
-        <v>36</v>
-      </c>
-      <c r="P12">
+      <c r="N12" s="19"/>
+      <c r="O12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P12" s="19">
         <v>11</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="19" t="s">
         <v>535</v>
       </c>
       <c r="R12" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
@@ -2813,6 +2899,9 @@
       <c r="C13" t="s">
         <v>19</v>
       </c>
+      <c r="D13" s="16">
+        <v>43084</v>
+      </c>
       <c r="E13" s="2">
         <v>42944</v>
       </c>
@@ -2822,8 +2911,8 @@
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="1">
-        <v>3</v>
+      <c r="I13" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>36</v>
@@ -2858,6 +2947,9 @@
       <c r="C14" t="s">
         <v>19</v>
       </c>
+      <c r="D14" s="16">
+        <v>43084</v>
+      </c>
       <c r="E14" s="2">
         <v>42945</v>
       </c>
@@ -2867,8 +2959,8 @@
       <c r="H14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="1">
-        <v>2</v>
+      <c r="I14" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>36</v>
@@ -2900,6 +2992,9 @@
       <c r="C15" t="s">
         <v>19</v>
       </c>
+      <c r="D15" s="16">
+        <v>43091</v>
+      </c>
       <c r="E15" s="2">
         <v>42946</v>
       </c>
@@ -2909,8 +3004,8 @@
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="1">
-        <v>4</v>
+      <c r="I15" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>36</v>
@@ -2951,8 +3046,8 @@
       <c r="H16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1">
-        <v>4</v>
+      <c r="I16" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>36</v>
@@ -2990,6 +3085,9 @@
       <c r="C17" t="s">
         <v>19</v>
       </c>
+      <c r="D17" s="16">
+        <v>43091</v>
+      </c>
       <c r="E17" s="2">
         <v>42947</v>
       </c>
@@ -2999,8 +3097,8 @@
       <c r="H17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="1">
-        <v>3</v>
+      <c r="I17" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>36</v>
@@ -3032,6 +3130,9 @@
       <c r="C18" t="s">
         <v>19</v>
       </c>
+      <c r="D18" s="16">
+        <v>43091</v>
+      </c>
       <c r="E18" s="2">
         <v>42948</v>
       </c>
@@ -3096,51 +3197,57 @@
         <f>[Date Breed]+114</f>
         <v>43063</v>
       </c>
-      <c r="M19"/>
       <c r="N19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1">
-      <c r="A20" t="s">
+      <c r="A20" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="C20" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="27">
         <v>42949</v>
       </c>
-      <c r="G20" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="F20" s="26"/>
+      <c r="G20" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" s="2">
+      <c r="J20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27">
         <f>[Date Breed]+114</f>
         <v>43063</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="29">
         <v>43429</v>
       </c>
-      <c r="O20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20">
+      <c r="N20" s="19"/>
+      <c r="O20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="P20" s="19">
         <v>8</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q20" s="19" t="s">
         <v>536</v>
+      </c>
+      <c r="R20" s="19" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1">
@@ -3153,6 +3260,9 @@
       <c r="C21" t="s">
         <v>19</v>
       </c>
+      <c r="D21" s="16">
+        <v>43091</v>
+      </c>
       <c r="E21" s="2">
         <v>42950</v>
       </c>
@@ -3195,6 +3305,9 @@
       <c r="C22" t="s">
         <v>19</v>
       </c>
+      <c r="D22" s="16">
+        <v>43099</v>
+      </c>
       <c r="E22" s="2">
         <v>42951</v>
       </c>
@@ -3259,7 +3372,6 @@
         <f>[Date Breed]+114</f>
         <v>43066</v>
       </c>
-      <c r="M23"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1">
       <c r="A24" t="s">
@@ -3271,6 +3383,9 @@
       <c r="C24" t="s">
         <v>19</v>
       </c>
+      <c r="D24" s="16">
+        <v>43099</v>
+      </c>
       <c r="E24" s="2">
         <v>42954</v>
       </c>
@@ -3332,12 +3447,11 @@
         <f>[Date Breed]+114</f>
         <v>43069</v>
       </c>
-      <c r="M25"/>
       <c r="N25" t="s">
         <v>30</v>
       </c>
       <c r="R25" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1">
@@ -3369,7 +3483,6 @@
         <f>[Date Breed]+114</f>
         <v>43071</v>
       </c>
-      <c r="M26"/>
       <c r="Q26" t="s">
         <v>540</v>
       </c>
@@ -3406,7 +3519,6 @@
         <f>[Date Breed]+114</f>
         <v>43071</v>
       </c>
-      <c r="M27"/>
       <c r="N27" t="s">
         <v>25</v>
       </c>
@@ -3421,6 +3533,9 @@
       <c r="C28" t="s">
         <v>19</v>
       </c>
+      <c r="D28" s="16">
+        <v>43099</v>
+      </c>
       <c r="E28" s="2">
         <v>42957</v>
       </c>
@@ -3466,6 +3581,9 @@
       <c r="C29" t="s">
         <v>19</v>
       </c>
+      <c r="D29" s="16">
+        <v>43099</v>
+      </c>
       <c r="E29" s="2">
         <v>42958</v>
       </c>
@@ -3508,6 +3626,9 @@
       <c r="C30" t="s">
         <v>19</v>
       </c>
+      <c r="D30" s="16">
+        <v>43099</v>
+      </c>
       <c r="E30" s="2">
         <v>42959</v>
       </c>
@@ -3537,7 +3658,7 @@
         <v>3</v>
       </c>
       <c r="Q30" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1">
@@ -3595,6 +3716,9 @@
       <c r="C32" t="s">
         <v>19</v>
       </c>
+      <c r="D32" s="16">
+        <v>43105</v>
+      </c>
       <c r="E32" s="2">
         <v>42961</v>
       </c>
@@ -3637,6 +3761,9 @@
       <c r="C33" t="s">
         <v>19</v>
       </c>
+      <c r="D33" s="16">
+        <v>43105</v>
+      </c>
       <c r="E33" s="2">
         <v>42961</v>
       </c>
@@ -3679,6 +3806,7 @@
       <c r="C34" t="s">
         <v>19</v>
       </c>
+      <c r="D34" s="16"/>
       <c r="E34" s="2">
         <v>42963</v>
       </c>
@@ -3701,7 +3829,6 @@
         <f>[Date Breed]+114</f>
         <v>43077</v>
       </c>
-      <c r="M34"/>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" t="s">
@@ -3735,7 +3862,6 @@
         <f>[Date Breed]+114</f>
         <v>43080</v>
       </c>
-      <c r="M35"/>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" t="s">
@@ -3769,7 +3895,6 @@
         <f>[Date Breed]+114</f>
         <v>43082</v>
       </c>
-      <c r="M36"/>
       <c r="N36" t="s">
         <v>28</v>
       </c>
@@ -3806,7 +3931,6 @@
         <f>[Date Breed]+114</f>
         <v>43083</v>
       </c>
-      <c r="M37"/>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" t="s">
@@ -3840,7 +3964,6 @@
         <f>[Date Breed]+114</f>
         <v>43085</v>
       </c>
-      <c r="M38"/>
       <c r="N38" t="s">
         <v>57</v>
       </c>
@@ -3877,7 +4000,6 @@
         <f>[Date Breed]+114</f>
         <v>43085</v>
       </c>
-      <c r="M39"/>
     </row>
     <row r="40" spans="1:18">
       <c r="A40" t="s">
@@ -3911,7 +4033,6 @@
         <f>[Date Breed]+114</f>
         <v>43086</v>
       </c>
-      <c r="M40"/>
       <c r="N40" t="s">
         <v>65</v>
       </c>
@@ -3948,7 +4069,6 @@
         <f>[Date Breed]+114</f>
         <v>43087</v>
       </c>
-      <c r="M41"/>
     </row>
     <row r="42" spans="1:18">
       <c r="A42" t="s">
@@ -3979,9 +4099,8 @@
         <f>[Date Breed]+114</f>
         <v>43087</v>
       </c>
-      <c r="M42"/>
       <c r="R42" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -4016,7 +4135,6 @@
         <f>[Date Breed]+114</f>
         <v>43090</v>
       </c>
-      <c r="M43"/>
     </row>
     <row r="44" spans="1:18">
       <c r="A44" t="s">
@@ -4050,7 +4168,6 @@
         <f>[Date Breed]+114</f>
         <v>43091</v>
       </c>
-      <c r="M44"/>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" t="s">
@@ -4084,7 +4201,6 @@
         <f>[Date Breed]+114</f>
         <v>43091</v>
       </c>
-      <c r="M45"/>
     </row>
     <row r="46" spans="1:18">
       <c r="A46" t="s">
@@ -4118,7 +4234,6 @@
         <f>[Date Breed]+114</f>
         <v>43093</v>
       </c>
-      <c r="M46"/>
       <c r="N46" t="s">
         <v>73</v>
       </c>
@@ -4155,7 +4270,6 @@
         <f>[Date Breed]+114</f>
         <v>43093</v>
       </c>
-      <c r="M47"/>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" t="s">
@@ -4189,7 +4303,6 @@
         <f>[Date Breed]+114</f>
         <v>43093</v>
       </c>
-      <c r="M48"/>
     </row>
     <row r="49" spans="1:17">
       <c r="A49" t="s">
@@ -4201,6 +4314,9 @@
       <c r="C49" t="s">
         <v>19</v>
       </c>
+      <c r="D49" s="16">
+        <v>43119</v>
+      </c>
       <c r="E49" s="2">
         <v>42980</v>
       </c>
@@ -4220,7 +4336,6 @@
         <f>[Date Breed]+114</f>
         <v>43094</v>
       </c>
-      <c r="M49"/>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" t="s">
@@ -4251,7 +4366,6 @@
         <f>[Date Breed]+114</f>
         <v>43093</v>
       </c>
-      <c r="M50"/>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" t="s">
@@ -4263,6 +4377,9 @@
       <c r="C51" t="s">
         <v>19</v>
       </c>
+      <c r="D51" s="16">
+        <v>43119</v>
+      </c>
       <c r="E51" s="2">
         <v>42980</v>
       </c>
@@ -4327,7 +4444,6 @@
         <f>[Date Breed]+114</f>
         <v>43094</v>
       </c>
-      <c r="M52"/>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" t="s">
@@ -4339,6 +4455,9 @@
       <c r="C53" t="s">
         <v>19</v>
       </c>
+      <c r="D53" s="16">
+        <v>43126</v>
+      </c>
       <c r="E53" s="2">
         <v>42982</v>
       </c>
@@ -4381,6 +4500,9 @@
       <c r="C54" t="s">
         <v>19</v>
       </c>
+      <c r="D54" s="16">
+        <v>43126</v>
+      </c>
       <c r="E54" s="2">
         <v>42985</v>
       </c>
@@ -4423,6 +4545,9 @@
       <c r="C55" t="s">
         <v>19</v>
       </c>
+      <c r="D55" s="16">
+        <v>43102</v>
+      </c>
       <c r="E55" s="2">
         <v>42985</v>
       </c>
@@ -4487,7 +4612,6 @@
         <f>[Date Breed]+114</f>
         <v>43099</v>
       </c>
-      <c r="M56"/>
     </row>
     <row r="57" spans="1:17">
       <c r="A57" t="s">
@@ -4499,6 +4623,9 @@
       <c r="C57" t="s">
         <v>19</v>
       </c>
+      <c r="D57" s="16">
+        <v>43133</v>
+      </c>
       <c r="E57" s="2">
         <v>42985</v>
       </c>
@@ -4544,6 +4671,9 @@
       <c r="C58" t="s">
         <v>19</v>
       </c>
+      <c r="D58" s="16">
+        <v>43138</v>
+      </c>
       <c r="E58" s="2">
         <v>42982</v>
       </c>
@@ -4566,7 +4696,6 @@
         <f>[Date Breed]+114</f>
         <v>43096</v>
       </c>
-      <c r="M58"/>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" t="s">
@@ -4607,7 +4736,7 @@
         <v>1</v>
       </c>
       <c r="Q59" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -4620,6 +4749,9 @@
       <c r="C60" t="s">
         <v>19</v>
       </c>
+      <c r="D60" s="16">
+        <v>43126</v>
+      </c>
       <c r="E60" s="2">
         <v>42989</v>
       </c>
@@ -4684,7 +4816,6 @@
         <f>[Date Breed]+114</f>
         <v>43103</v>
       </c>
-      <c r="M61"/>
       <c r="N61" t="s">
         <v>88</v>
       </c>
@@ -4699,6 +4830,9 @@
       <c r="C62" t="s">
         <v>19</v>
       </c>
+      <c r="D62" s="16">
+        <v>43133</v>
+      </c>
       <c r="E62" s="2">
         <v>42989</v>
       </c>
@@ -4760,7 +4894,6 @@
         <f>[Date Breed]+114</f>
         <v>43103</v>
       </c>
-      <c r="M63"/>
       <c r="N63" t="s">
         <v>90</v>
       </c>
@@ -4797,12 +4930,11 @@
         <f>[Date Breed]+114</f>
         <v>43104</v>
       </c>
-      <c r="M64"/>
       <c r="N64" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:18">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -4812,6 +4944,9 @@
       <c r="C65" t="s">
         <v>19</v>
       </c>
+      <c r="D65" s="16">
+        <v>43133</v>
+      </c>
       <c r="E65" s="2">
         <v>42990</v>
       </c>
@@ -4847,7 +4982,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:18">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -4876,7 +5011,7 @@
         <f>[Date Breed]+114</f>
         <v>43105</v>
       </c>
-      <c r="M66" s="2">
+      <c r="M66" s="16">
         <v>43106</v>
       </c>
       <c r="O66" t="s">
@@ -4886,10 +5021,10 @@
         <v>4</v>
       </c>
       <c r="Q66" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -4899,6 +5034,9 @@
       <c r="C67" t="s">
         <v>19</v>
       </c>
+      <c r="D67" s="16">
+        <v>43138</v>
+      </c>
       <c r="E67" s="2">
         <v>42991</v>
       </c>
@@ -4931,10 +5069,10 @@
         <v>3</v>
       </c>
       <c r="Q67" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68" t="s">
         <v>144</v>
       </c>
@@ -4944,6 +5082,7 @@
       <c r="C68" t="s">
         <v>19</v>
       </c>
+      <c r="D68" s="16"/>
       <c r="E68" s="2">
         <v>42991</v>
       </c>
@@ -4976,10 +5115,11 @@
         <v>4</v>
       </c>
       <c r="Q68" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17">
+        <v>585</v>
+      </c>
+      <c r="R68" s="16"/>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69" t="s">
         <v>145</v>
       </c>
@@ -4989,6 +5129,9 @@
       <c r="C69" t="s">
         <v>19</v>
       </c>
+      <c r="D69" s="16">
+        <v>43133</v>
+      </c>
       <c r="E69" s="2">
         <v>42991</v>
       </c>
@@ -5021,7 +5164,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:18">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -5050,9 +5193,8 @@
         <f>[Date Breed]+114</f>
         <v>43105</v>
       </c>
-      <c r="M70"/>
-    </row>
-    <row r="71" spans="1:17">
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -5084,9 +5226,8 @@
         <f>[Date Breed]+114</f>
         <v>43107</v>
       </c>
-      <c r="M71"/>
-    </row>
-    <row r="72" spans="1:17">
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -5096,6 +5237,9 @@
       <c r="C72" t="s">
         <v>19</v>
       </c>
+      <c r="D72" s="16">
+        <v>43138</v>
+      </c>
       <c r="E72" s="2">
         <v>42994</v>
       </c>
@@ -5125,10 +5269,10 @@
         <v>14</v>
       </c>
       <c r="Q72" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -5160,9 +5304,8 @@
         <f>[Date Breed]+114</f>
         <v>43108</v>
       </c>
-      <c r="M73"/>
-    </row>
-    <row r="74" spans="1:17">
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74" t="s">
         <v>155</v>
       </c>
@@ -5191,12 +5334,11 @@
         <f>[Date Breed]+114</f>
         <v>43111</v>
       </c>
-      <c r="M74"/>
       <c r="N74" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:18">
       <c r="A75" t="s">
         <v>156</v>
       </c>
@@ -5225,12 +5367,11 @@
         <f>[Date Breed]+114</f>
         <v>43111</v>
       </c>
-      <c r="M75"/>
       <c r="N75" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:18">
       <c r="A76" t="s">
         <v>157</v>
       </c>
@@ -5259,9 +5400,8 @@
         <f>[Date Breed]+114</f>
         <v>43111</v>
       </c>
-      <c r="M76"/>
-    </row>
-    <row r="77" spans="1:17">
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -5271,6 +5411,9 @@
       <c r="C77" t="s">
         <v>19</v>
       </c>
+      <c r="D77" s="16">
+        <v>43138</v>
+      </c>
       <c r="E77" s="2">
         <v>42997</v>
       </c>
@@ -5303,7 +5446,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:18">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -5313,6 +5456,9 @@
       <c r="C78" t="s">
         <v>19</v>
       </c>
+      <c r="D78" s="16">
+        <v>43138</v>
+      </c>
       <c r="E78" s="2">
         <v>42999</v>
       </c>
@@ -5345,7 +5491,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:18">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -5355,6 +5501,9 @@
       <c r="C79" t="s">
         <v>19</v>
       </c>
+      <c r="D79" s="16">
+        <v>43144</v>
+      </c>
       <c r="E79" s="2">
         <v>42999</v>
       </c>
@@ -5387,7 +5536,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:18">
       <c r="A80" t="s">
         <v>165</v>
       </c>
@@ -5416,7 +5565,6 @@
         <f>[Date Breed]+114</f>
         <v>43113</v>
       </c>
-      <c r="M80"/>
     </row>
     <row r="81" spans="1:17">
       <c r="A81" t="s">
@@ -5428,6 +5576,9 @@
       <c r="C81" t="s">
         <v>19</v>
       </c>
+      <c r="D81" s="16">
+        <v>43138</v>
+      </c>
       <c r="E81" s="2">
         <v>43000</v>
       </c>
@@ -5473,6 +5624,9 @@
       <c r="C82" t="s">
         <v>19</v>
       </c>
+      <c r="D82" s="16">
+        <v>43144</v>
+      </c>
       <c r="E82" s="2">
         <v>43000</v>
       </c>
@@ -5518,6 +5672,9 @@
       <c r="C83" t="s">
         <v>19</v>
       </c>
+      <c r="D83" s="16">
+        <v>43144</v>
+      </c>
       <c r="E83" s="2">
         <v>43001</v>
       </c>
@@ -5579,7 +5736,6 @@
         <f>[Date Breed]+114</f>
         <v>43115</v>
       </c>
-      <c r="M84"/>
     </row>
     <row r="85" spans="1:17">
       <c r="A85" t="s">
@@ -5610,7 +5766,6 @@
         <f>[Date Breed]+114</f>
         <v>43115</v>
       </c>
-      <c r="M85"/>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" t="s">
@@ -5641,7 +5796,6 @@
         <f>[Date Breed]+114</f>
         <v>43116</v>
       </c>
-      <c r="M86"/>
       <c r="N86" t="s">
         <v>122</v>
       </c>
@@ -5675,7 +5829,6 @@
         <f>[Date Breed]+114</f>
         <v>43116</v>
       </c>
-      <c r="M87"/>
     </row>
     <row r="88" spans="1:17">
       <c r="A88" t="s">
@@ -5706,7 +5859,6 @@
         <f>[Date Breed]+114</f>
         <v>43116</v>
       </c>
-      <c r="M88"/>
     </row>
     <row r="89" spans="1:17">
       <c r="A89" t="s">
@@ -5718,6 +5870,9 @@
       <c r="C89" t="s">
         <v>19</v>
       </c>
+      <c r="D89" s="16">
+        <v>43144</v>
+      </c>
       <c r="E89" s="2">
         <v>43003</v>
       </c>
@@ -5737,7 +5892,9 @@
         <f>[Date Breed]+114</f>
         <v>43117</v>
       </c>
-      <c r="M89"/>
+      <c r="M89" s="16">
+        <v>43115</v>
+      </c>
       <c r="N89" t="s">
         <v>109</v>
       </c>
@@ -5784,7 +5941,7 @@
         <v>17</v>
       </c>
       <c r="Q90" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -5797,6 +5954,9 @@
       <c r="C91" t="s">
         <v>19</v>
       </c>
+      <c r="D91" s="16">
+        <v>43152</v>
+      </c>
       <c r="E91" s="2">
         <v>43005</v>
       </c>
@@ -5816,7 +5976,6 @@
         <f>[Date Breed]+114</f>
         <v>43119</v>
       </c>
-      <c r="M91"/>
     </row>
     <row r="92" spans="1:17">
       <c r="A92" t="s">
@@ -5828,6 +5987,9 @@
       <c r="C92" t="s">
         <v>19</v>
       </c>
+      <c r="D92" s="16">
+        <v>43152</v>
+      </c>
       <c r="E92" s="2">
         <v>43009</v>
       </c>
@@ -5895,7 +6057,6 @@
         <f>[Date Breed]+114</f>
         <v>43124</v>
       </c>
-      <c r="M93"/>
     </row>
     <row r="94" spans="1:17">
       <c r="A94" t="s">
@@ -5907,6 +6068,9 @@
       <c r="C94" t="s">
         <v>19</v>
       </c>
+      <c r="D94" s="16">
+        <v>43152</v>
+      </c>
       <c r="E94" s="2">
         <v>43010</v>
       </c>
@@ -5949,6 +6113,9 @@
       <c r="C95" t="s">
         <v>19</v>
       </c>
+      <c r="D95" s="16">
+        <v>43152</v>
+      </c>
       <c r="E95" s="2">
         <v>43010</v>
       </c>
@@ -5968,9 +6135,17 @@
         <f>[Date Breed]+114</f>
         <v>43124</v>
       </c>
-      <c r="M95"/>
+      <c r="M95" s="16">
+        <v>43123</v>
+      </c>
       <c r="N95" t="s">
         <v>128</v>
+      </c>
+      <c r="P95">
+        <v>9</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="96" spans="1:17">
@@ -5983,6 +6158,9 @@
       <c r="C96" t="s">
         <v>19</v>
       </c>
+      <c r="D96" s="16">
+        <v>43152</v>
+      </c>
       <c r="E96" s="2">
         <v>43012</v>
       </c>
@@ -6028,6 +6206,9 @@
       <c r="C97" t="s">
         <v>19</v>
       </c>
+      <c r="D97" s="16">
+        <v>43152</v>
+      </c>
       <c r="E97" s="2">
         <v>43013</v>
       </c>
@@ -6070,6 +6251,9 @@
       <c r="C98" t="s">
         <v>19</v>
       </c>
+      <c r="D98" s="16">
+        <v>43161</v>
+      </c>
       <c r="E98" s="2">
         <v>43014</v>
       </c>
@@ -6102,7 +6286,7 @@
         <v>0</v>
       </c>
       <c r="Q98" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="99" spans="1:18">
@@ -6115,6 +6299,9 @@
       <c r="C99" t="s">
         <v>19</v>
       </c>
+      <c r="D99" s="16">
+        <v>43161</v>
+      </c>
       <c r="E99" s="2">
         <v>43015</v>
       </c>
@@ -6157,6 +6344,9 @@
       <c r="C100" t="s">
         <v>19</v>
       </c>
+      <c r="D100" s="16">
+        <v>43161</v>
+      </c>
       <c r="E100" s="2">
         <v>43016</v>
       </c>
@@ -6202,6 +6392,9 @@
       <c r="C101" t="s">
         <v>19</v>
       </c>
+      <c r="D101" s="16">
+        <v>43168</v>
+      </c>
       <c r="E101" s="2">
         <v>43017</v>
       </c>
@@ -6244,6 +6437,7 @@
       <c r="C102" t="s">
         <v>19</v>
       </c>
+      <c r="D102" s="16"/>
       <c r="E102" s="2">
         <v>43017</v>
       </c>
@@ -6263,7 +6457,6 @@
         <f>[Date Breed]+114</f>
         <v>43131</v>
       </c>
-      <c r="M102"/>
     </row>
     <row r="103" spans="1:18">
       <c r="A103" t="s">
@@ -6275,6 +6468,9 @@
       <c r="C103" t="s">
         <v>19</v>
       </c>
+      <c r="D103" s="16">
+        <v>43161</v>
+      </c>
       <c r="E103" s="2">
         <v>43018</v>
       </c>
@@ -6339,7 +6535,6 @@
         <f>[Date Breed]+114</f>
         <v>43133</v>
       </c>
-      <c r="M104"/>
       <c r="N104" t="s">
         <v>108</v>
       </c>
@@ -6373,7 +6568,6 @@
         <f>[Date Breed]+114</f>
         <v>43134</v>
       </c>
-      <c r="M105"/>
       <c r="N105" t="s">
         <v>176</v>
       </c>
@@ -6388,6 +6582,9 @@
       <c r="C106" t="s">
         <v>19</v>
       </c>
+      <c r="D106" s="16">
+        <v>43168</v>
+      </c>
       <c r="E106" s="2">
         <v>43022</v>
       </c>
@@ -6452,7 +6649,6 @@
         <f>[Date Breed]+114</f>
         <v>43136</v>
       </c>
-      <c r="M107"/>
       <c r="N107" t="s">
         <v>165</v>
       </c>
@@ -6531,7 +6727,6 @@
         <f>[Date Breed]+114</f>
         <v>43137</v>
       </c>
-      <c r="M109"/>
       <c r="N109" t="s">
         <v>179</v>
       </c>
@@ -6546,6 +6741,9 @@
       <c r="C110" t="s">
         <v>19</v>
       </c>
+      <c r="D110" s="16">
+        <v>43168</v>
+      </c>
       <c r="E110" s="2">
         <v>43024</v>
       </c>
@@ -6604,12 +6802,11 @@
         <f>[Date Breed]+114</f>
         <v>43139</v>
       </c>
-      <c r="M111"/>
       <c r="N111" t="s">
         <v>113</v>
       </c>
       <c r="R111" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="112" spans="1:18">
@@ -6641,7 +6838,6 @@
         <f>[Date Breed]+114</f>
         <v>43139</v>
       </c>
-      <c r="M112"/>
       <c r="N112" t="s">
         <v>111</v>
       </c>
@@ -6685,7 +6881,7 @@
         <v>0</v>
       </c>
       <c r="Q113" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="114" spans="1:18" ht="15" customHeight="1">
@@ -6717,7 +6913,6 @@
         <f>[Date Breed]+114</f>
         <v>43139</v>
       </c>
-      <c r="M114"/>
       <c r="N114" t="s">
         <v>183</v>
       </c>
@@ -6732,6 +6927,9 @@
       <c r="C115" t="s">
         <v>19</v>
       </c>
+      <c r="D115" s="16">
+        <v>43168</v>
+      </c>
       <c r="E115" s="2">
         <v>43026</v>
       </c>
@@ -6774,6 +6972,9 @@
       <c r="C116" t="s">
         <v>19</v>
       </c>
+      <c r="D116" s="16">
+        <v>43175</v>
+      </c>
       <c r="E116" s="2">
         <v>43027</v>
       </c>
@@ -6803,7 +7004,7 @@
         <v>13</v>
       </c>
       <c r="Q116" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="117" spans="1:18" ht="15" customHeight="1">
@@ -6848,7 +7049,7 @@
         <v>1</v>
       </c>
       <c r="Q117" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="118" spans="1:18" ht="15" customHeight="1">
@@ -6861,6 +7062,9 @@
       <c r="C118" t="s">
         <v>19</v>
       </c>
+      <c r="D118" s="16">
+        <v>43175</v>
+      </c>
       <c r="E118" s="2">
         <v>43028</v>
       </c>
@@ -6906,6 +7110,9 @@
       <c r="C119" t="s">
         <v>19</v>
       </c>
+      <c r="D119" s="16">
+        <v>43175</v>
+      </c>
       <c r="E119" s="2">
         <v>43028</v>
       </c>
@@ -6938,7 +7145,7 @@
         <v>13</v>
       </c>
       <c r="Q119" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="120" spans="1:18">
@@ -6980,7 +7187,7 @@
         <v>15</v>
       </c>
       <c r="Q120" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="121" spans="1:18">
@@ -7023,7 +7230,7 @@
       <c r="P121" s="4"/>
       <c r="Q121" s="4"/>
       <c r="R121" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="122" spans="1:18">
@@ -7066,7 +7273,7 @@
       <c r="P122" s="4"/>
       <c r="Q122" s="4"/>
       <c r="R122" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="123" spans="1:18">
@@ -7290,7 +7497,7 @@
         <v>3</v>
       </c>
       <c r="Q127" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="128" spans="1:18">
@@ -7382,7 +7589,7 @@
         <v>3</v>
       </c>
       <c r="Q129" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="130" spans="1:17">
@@ -7428,7 +7635,7 @@
         <v>1</v>
       </c>
       <c r="Q130" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="131" spans="1:17">
@@ -8252,10 +8459,10 @@
         <v>14</v>
       </c>
       <c r="Q149" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="R149" s="19" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="150" spans="1:18">
@@ -8346,7 +8553,7 @@
       <c r="A152" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="22" t="s">
         <v>180</v>
       </c>
       <c r="C152" s="4" t="s">
@@ -8374,11 +8581,19 @@
         <f>[Date Breed]+114</f>
         <v>43176</v>
       </c>
-      <c r="M152" s="4"/>
+      <c r="M152" s="21">
+        <v>43178</v>
+      </c>
       <c r="N152" s="4"/>
-      <c r="O152" s="4"/>
-      <c r="P152" s="4"/>
-      <c r="Q152" s="4"/>
+      <c r="O152" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P152" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q152" s="4" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="153" spans="1:18">
       <c r="A153" s="4" t="s">
@@ -8417,7 +8632,7 @@
       </c>
       <c r="N153" s="4"/>
       <c r="O153" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="P153" s="4">
         <v>11</v>
@@ -8430,7 +8645,7 @@
       <c r="A154" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="22" t="s">
         <v>184</v>
       </c>
       <c r="C154" s="4" t="s">
@@ -8458,17 +8673,25 @@
         <f>[Date Breed]+114</f>
         <v>43176</v>
       </c>
-      <c r="M154" s="4"/>
+      <c r="M154" s="21">
+        <v>43179</v>
+      </c>
       <c r="N154" s="4"/>
-      <c r="O154" s="4"/>
-      <c r="P154" s="4"/>
-      <c r="Q154" s="4"/>
+      <c r="O154" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="P154" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q154" s="4" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="155" spans="1:18">
       <c r="A155" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B155" s="22" t="s">
         <v>287</v>
       </c>
       <c r="C155" s="4" t="s">
@@ -8496,17 +8719,23 @@
         <f>[Date Breed]+114</f>
         <v>43179</v>
       </c>
-      <c r="M155" s="4"/>
+      <c r="M155" s="21">
+        <v>43181</v>
+      </c>
       <c r="N155" s="4"/>
       <c r="O155" s="4"/>
-      <c r="P155" s="4"/>
-      <c r="Q155" s="4"/>
+      <c r="P155" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q155" s="4" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="156" spans="1:18">
       <c r="A156" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="22" t="s">
         <v>289</v>
       </c>
       <c r="C156" s="4" t="s">
@@ -8534,11 +8763,17 @@
         <f>[Date Breed]+114</f>
         <v>43178</v>
       </c>
-      <c r="M156" s="4"/>
+      <c r="M156" s="21">
+        <v>43181</v>
+      </c>
       <c r="N156" s="4"/>
       <c r="O156" s="4"/>
-      <c r="P156" s="4"/>
-      <c r="Q156" s="4"/>
+      <c r="P156" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q156" s="4" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="157" spans="1:18">
       <c r="A157" s="4" t="s">
@@ -9228,7 +9463,7 @@
       <c r="P174" s="4"/>
       <c r="Q174" s="4"/>
       <c r="R174" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="175" spans="1:18">
@@ -10497,7 +10732,7 @@
       <c r="P207" s="4"/>
       <c r="Q207" s="4"/>
       <c r="R207" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="208" spans="1:18">
@@ -12476,7 +12711,7 @@
       <c r="P259" s="4"/>
       <c r="Q259" s="4"/>
       <c r="R259" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="260" spans="1:18">
@@ -12517,7 +12752,7 @@
       <c r="P260" s="4"/>
       <c r="Q260" s="4"/>
       <c r="R260" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="261" spans="1:18">
@@ -12625,7 +12860,6 @@
         <f>[Date Breed]+114</f>
         <v>43246</v>
       </c>
-      <c r="M263"/>
     </row>
     <row r="264" spans="1:18">
       <c r="A264" s="4" t="s">
@@ -12656,7 +12890,6 @@
         <f>[Date Breed]+114</f>
         <v>43246</v>
       </c>
-      <c r="M264"/>
     </row>
     <row r="265" spans="1:18">
       <c r="A265" s="4" t="s">
@@ -12687,7 +12920,6 @@
         <f>[Date Breed]+114</f>
         <v>43247</v>
       </c>
-      <c r="M265"/>
     </row>
     <row r="266" spans="1:18">
       <c r="A266" s="4" t="s">
@@ -12718,7 +12950,6 @@
         <f>[Date Breed]+114</f>
         <v>43247</v>
       </c>
-      <c r="M266"/>
     </row>
     <row r="267" spans="1:18">
       <c r="A267" s="4" t="s">
@@ -12749,7 +12980,6 @@
         <f>[Date Breed]+114</f>
         <v>43249</v>
       </c>
-      <c r="M267"/>
     </row>
     <row r="268" spans="1:18">
       <c r="A268" s="4" t="s">
@@ -12780,7 +13010,6 @@
         <f>[Date Breed]+114</f>
         <v>43249</v>
       </c>
-      <c r="M268"/>
     </row>
     <row r="269" spans="1:18">
       <c r="A269" s="4" t="s">
@@ -12811,7 +13040,6 @@
         <f>[Date Breed]+114</f>
         <v>43250</v>
       </c>
-      <c r="M269"/>
     </row>
     <row r="270" spans="1:18">
       <c r="A270" s="4" t="s">
@@ -12842,7 +13070,6 @@
         <f>[Date Breed]+114</f>
         <v>43251</v>
       </c>
-      <c r="M270"/>
     </row>
     <row r="271" spans="1:18">
       <c r="A271" s="4" t="s">
@@ -13077,7 +13304,7 @@
         <v>467</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C277" s="4" t="s">
         <v>19</v>
@@ -13115,7 +13342,7 @@
         <v>468</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C278" s="4" t="s">
         <v>19</v>
@@ -13191,7 +13418,7 @@
         <v>470</v>
       </c>
       <c r="B280" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C280" s="11" t="s">
         <v>19</v>
@@ -13229,7 +13456,7 @@
         <v>471</v>
       </c>
       <c r="B281" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C281" s="11" t="s">
         <v>19</v>
@@ -13381,7 +13608,7 @@
         <v>475</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C285" s="4" t="s">
         <v>19</v>
@@ -13414,7 +13641,7 @@
       <c r="P285" s="4"/>
       <c r="Q285" s="4"/>
       <c r="R285" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="286" spans="1:18">
@@ -13536,7 +13763,7 @@
         <v>479</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C289" s="4" t="s">
         <v>19</v>
@@ -13650,7 +13877,7 @@
         <v>482</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C292" s="4" t="s">
         <v>19</v>
@@ -13688,7 +13915,7 @@
         <v>483</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C293" s="4" t="s">
         <v>19</v>
@@ -13726,7 +13953,7 @@
         <v>484</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C294" s="4" t="s">
         <v>19</v>
@@ -13740,7 +13967,7 @@
         <v>20</v>
       </c>
       <c r="H294" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I294" s="5" t="s">
         <v>60</v>
@@ -13778,7 +14005,7 @@
         <v>20</v>
       </c>
       <c r="H295" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I295" s="5" t="s">
         <v>60</v>
@@ -13859,7 +14086,9 @@
       <c r="I297" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J297" s="9"/>
+      <c r="J297" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="K297" s="8"/>
       <c r="L297" s="8">
         <f>[Date Breed]+114</f>
@@ -13895,7 +14124,9 @@
       <c r="I298" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J298" s="9"/>
+      <c r="J298" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="K298" s="8"/>
       <c r="L298" s="8">
         <f>[Date Breed]+114</f>
@@ -13931,7 +14162,9 @@
       <c r="I299" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J299" s="9"/>
+      <c r="J299" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="K299" s="8"/>
       <c r="L299" s="8">
         <f>[Date Breed]+114</f>
@@ -13948,7 +14181,7 @@
         <v>490</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C300" s="4" t="s">
         <v>19</v>
@@ -13967,7 +14200,9 @@
       <c r="I300" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J300" s="9"/>
+      <c r="J300" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="K300" s="8"/>
       <c r="L300" s="8">
         <f>[Date Breed]+114</f>
@@ -14003,7 +14238,9 @@
       <c r="I301" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J301" s="9"/>
+      <c r="J301" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="K301" s="8"/>
       <c r="L301" s="8">
         <f>[Date Breed]+114</f>
@@ -14056,7 +14293,7 @@
         <v>493</v>
       </c>
       <c r="B303" s="10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C303" s="11" t="s">
         <v>19</v>
@@ -14164,7 +14401,7 @@
         <v>496</v>
       </c>
       <c r="B306" s="10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C306" s="11" t="s">
         <v>19</v>
@@ -14700,22 +14937,34 @@
       <c r="Q320" s="4"/>
     </row>
     <row r="321" spans="1:17">
-      <c r="A321" s="4" t="s">
+      <c r="A321" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="B321" s="5"/>
-      <c r="C321" s="4"/>
-      <c r="D321" s="4"/>
-      <c r="E321" s="8"/>
-      <c r="F321" s="5"/>
-      <c r="G321" s="24"/>
-      <c r="H321" s="5"/>
-      <c r="I321" s="5"/>
-      <c r="J321" s="9"/>
-      <c r="K321" s="8"/>
-      <c r="L321" s="8">
-        <f>[Date Breed]+114</f>
-        <v>114</v>
+      <c r="B321" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="C321" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D321" s="11"/>
+      <c r="E321" s="12">
+        <v>43175</v>
+      </c>
+      <c r="F321" s="10"/>
+      <c r="G321" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H321" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="I321" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J321" s="13"/>
+      <c r="K321" s="12"/>
+      <c r="L321" s="12">
+        <f>[Date Breed]+114</f>
+        <v>43289</v>
       </c>
       <c r="M321" s="4"/>
       <c r="N321" s="4"/>
@@ -14724,22 +14973,34 @@
       <c r="Q321" s="4"/>
     </row>
     <row r="322" spans="1:17">
-      <c r="A322" s="4" t="s">
+      <c r="A322" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="B322" s="5"/>
-      <c r="C322" s="4"/>
-      <c r="D322" s="4"/>
-      <c r="E322" s="8"/>
-      <c r="F322" s="5"/>
-      <c r="G322" s="24"/>
-      <c r="H322" s="5"/>
-      <c r="I322" s="5"/>
-      <c r="J322" s="9"/>
-      <c r="K322" s="8"/>
-      <c r="L322" s="8">
-        <f>[Date Breed]+114</f>
-        <v>114</v>
+      <c r="B322" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="C322" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D322" s="11"/>
+      <c r="E322" s="12">
+        <v>43176</v>
+      </c>
+      <c r="F322" s="10"/>
+      <c r="G322" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H322" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="I322" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J322" s="13"/>
+      <c r="K322" s="12"/>
+      <c r="L322" s="12">
+        <f>[Date Breed]+114</f>
+        <v>43290</v>
       </c>
       <c r="M322" s="4"/>
       <c r="N322" s="4"/>
@@ -14751,19 +15012,31 @@
       <c r="A323" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="B323" s="5"/>
-      <c r="C323" s="4"/>
+      <c r="B323" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="C323" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D323" s="4"/>
-      <c r="E323" s="8"/>
+      <c r="E323" s="8">
+        <v>43176</v>
+      </c>
       <c r="F323" s="5"/>
-      <c r="G323" s="24"/>
-      <c r="H323" s="5"/>
-      <c r="I323" s="5"/>
+      <c r="G323" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H323" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I323" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J323" s="9"/>
       <c r="K323" s="8"/>
       <c r="L323" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43290</v>
       </c>
       <c r="M323" s="4"/>
       <c r="N323" s="4"/>
@@ -14775,19 +15048,31 @@
       <c r="A324" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="B324" s="5"/>
-      <c r="C324" s="4"/>
+      <c r="B324" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C324" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D324" s="4"/>
-      <c r="E324" s="8"/>
+      <c r="E324" s="8">
+        <v>43178</v>
+      </c>
       <c r="F324" s="5"/>
-      <c r="G324" s="24"/>
-      <c r="H324" s="5"/>
-      <c r="I324" s="5"/>
+      <c r="G324" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H324" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I324" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="J324" s="9"/>
       <c r="K324" s="8"/>
       <c r="L324" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43292</v>
       </c>
       <c r="M324" s="4"/>
       <c r="N324" s="4"/>
@@ -14799,19 +15084,31 @@
       <c r="A325" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="B325" s="5"/>
-      <c r="C325" s="4"/>
+      <c r="B325" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C325" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D325" s="4"/>
-      <c r="E325" s="8"/>
+      <c r="E325" s="8">
+        <v>43178</v>
+      </c>
       <c r="F325" s="5"/>
-      <c r="G325" s="24"/>
-      <c r="H325" s="5"/>
-      <c r="I325" s="5"/>
+      <c r="G325" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H325" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I325" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="J325" s="9"/>
       <c r="K325" s="8"/>
       <c r="L325" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43292</v>
       </c>
       <c r="M325" s="4"/>
       <c r="N325" s="4"/>
@@ -14823,19 +15120,31 @@
       <c r="A326" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="B326" s="5"/>
-      <c r="C326" s="4"/>
+      <c r="B326" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C326" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D326" s="4"/>
-      <c r="E326" s="8"/>
+      <c r="E326" s="8">
+        <v>43178</v>
+      </c>
       <c r="F326" s="5"/>
-      <c r="G326" s="24"/>
-      <c r="H326" s="5"/>
-      <c r="I326" s="5"/>
+      <c r="G326" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H326" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I326" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J326" s="9"/>
       <c r="K326" s="8"/>
       <c r="L326" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43292</v>
       </c>
       <c r="M326" s="4"/>
       <c r="N326" s="4"/>
@@ -14847,19 +15156,31 @@
       <c r="A327" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="B327" s="5"/>
-      <c r="C327" s="4"/>
+      <c r="B327" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C327" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D327" s="4"/>
-      <c r="E327" s="8"/>
+      <c r="E327" s="8">
+        <v>43179</v>
+      </c>
       <c r="F327" s="5"/>
-      <c r="G327" s="24"/>
-      <c r="H327" s="5"/>
-      <c r="I327" s="5"/>
+      <c r="G327" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H327" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I327" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J327" s="9"/>
       <c r="K327" s="8"/>
       <c r="L327" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43293</v>
       </c>
       <c r="M327" s="4"/>
       <c r="N327" s="4"/>
@@ -14871,19 +15192,31 @@
       <c r="A328" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="B328" s="5"/>
-      <c r="C328" s="4"/>
+      <c r="B328" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C328" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D328" s="4"/>
-      <c r="E328" s="8"/>
+      <c r="E328" s="8">
+        <v>43180</v>
+      </c>
       <c r="F328" s="5"/>
-      <c r="G328" s="24"/>
-      <c r="H328" s="5"/>
-      <c r="I328" s="5"/>
+      <c r="G328" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H328" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I328" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J328" s="9"/>
       <c r="K328" s="8"/>
       <c r="L328" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43294</v>
       </c>
       <c r="M328" s="4"/>
       <c r="N328" s="4"/>
@@ -14895,19 +15228,31 @@
       <c r="A329" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="B329" s="5"/>
-      <c r="C329" s="4"/>
+      <c r="B329" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C329" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D329" s="4"/>
-      <c r="E329" s="8"/>
+      <c r="E329" s="8">
+        <v>43180</v>
+      </c>
       <c r="F329" s="5"/>
-      <c r="G329" s="24"/>
-      <c r="H329" s="5"/>
-      <c r="I329" s="5"/>
+      <c r="G329" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H329" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I329" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J329" s="9"/>
       <c r="K329" s="8"/>
       <c r="L329" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43294</v>
       </c>
       <c r="M329" s="4"/>
       <c r="N329" s="4"/>
@@ -14919,19 +15264,31 @@
       <c r="A330" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="B330" s="5"/>
-      <c r="C330" s="4"/>
+      <c r="B330" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C330" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D330" s="4"/>
-      <c r="E330" s="8"/>
+      <c r="E330" s="8">
+        <v>43180</v>
+      </c>
       <c r="F330" s="5"/>
-      <c r="G330" s="24"/>
-      <c r="H330" s="5"/>
-      <c r="I330" s="5"/>
+      <c r="G330" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H330" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I330" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J330" s="9"/>
       <c r="K330" s="8"/>
       <c r="L330" s="8">
         <f>[Date Breed]+114</f>
-        <v>114</v>
+        <v>43294</v>
       </c>
       <c r="M330" s="4"/>
       <c r="N330" s="4"/>
@@ -15108,140 +15465,180 @@
       <c r="Q337" s="4"/>
     </row>
     <row r="338" spans="1:17">
+      <c r="A338" s="4" t="s">
+        <v>564</v>
+      </c>
       <c r="L338" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M338"/>
     </row>
     <row r="339" spans="1:17">
+      <c r="A339" s="4" t="s">
+        <v>565</v>
+      </c>
       <c r="L339" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M339"/>
     </row>
     <row r="340" spans="1:17">
+      <c r="A340" s="4" t="s">
+        <v>566</v>
+      </c>
       <c r="L340" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M340"/>
     </row>
     <row r="341" spans="1:17">
+      <c r="A341" s="4" t="s">
+        <v>567</v>
+      </c>
       <c r="L341" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M341"/>
     </row>
     <row r="342" spans="1:17">
+      <c r="A342" s="4" t="s">
+        <v>568</v>
+      </c>
       <c r="L342" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M342"/>
     </row>
     <row r="343" spans="1:17">
+      <c r="A343" s="4" t="s">
+        <v>569</v>
+      </c>
       <c r="L343" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M343"/>
     </row>
     <row r="344" spans="1:17">
+      <c r="A344" s="4" t="s">
+        <v>570</v>
+      </c>
       <c r="L344" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M344"/>
     </row>
     <row r="345" spans="1:17">
+      <c r="A345" s="4" t="s">
+        <v>571</v>
+      </c>
       <c r="L345" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M345"/>
     </row>
     <row r="346" spans="1:17">
+      <c r="A346" s="4" t="s">
+        <v>572</v>
+      </c>
       <c r="L346" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M346"/>
     </row>
     <row r="347" spans="1:17">
+      <c r="A347" s="4" t="s">
+        <v>573</v>
+      </c>
       <c r="L347" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M347"/>
     </row>
     <row r="348" spans="1:17">
+      <c r="A348" s="4" t="s">
+        <v>574</v>
+      </c>
       <c r="L348" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M348"/>
     </row>
     <row r="349" spans="1:17">
+      <c r="A349" s="4" t="s">
+        <v>575</v>
+      </c>
       <c r="L349" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M349"/>
     </row>
     <row r="350" spans="1:17">
+      <c r="A350" s="4" t="s">
+        <v>576</v>
+      </c>
       <c r="L350" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M350"/>
     </row>
     <row r="351" spans="1:17">
+      <c r="A351" s="4" t="s">
+        <v>577</v>
+      </c>
       <c r="L351" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M351"/>
     </row>
     <row r="352" spans="1:17">
+      <c r="A352" s="4" t="s">
+        <v>578</v>
+      </c>
       <c r="L352" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M352"/>
     </row>
     <row r="353" spans="1:18">
+      <c r="A353" s="4" t="s">
+        <v>579</v>
+      </c>
       <c r="L353" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M353"/>
     </row>
     <row r="354" spans="1:18">
+      <c r="A354" s="4" t="s">
+        <v>580</v>
+      </c>
       <c r="L354" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M354"/>
     </row>
     <row r="355" spans="1:18">
+      <c r="A355" s="4" t="s">
+        <v>581</v>
+      </c>
       <c r="L355" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M355"/>
     </row>
     <row r="356" spans="1:18">
+      <c r="A356" s="4" t="s">
+        <v>582</v>
+      </c>
       <c r="L356" s="2">
         <f>[Date Breed]+114</f>
         <v>114</v>
       </c>
-      <c r="M356"/>
     </row>
     <row r="357" spans="1:18">
-      <c r="A357" s="4"/>
+      <c r="A357" s="4" t="s">
+        <v>583</v>
+      </c>
       <c r="B357" s="5"/>
       <c r="C357" s="4"/>
       <c r="D357" s="4"/>

</xml_diff>